<commit_message>
feat: Add Monster MoveSpeedWave Component, MoveSpeed Balance fix
</commit_message>
<xml_diff>
--- a/INFEST_Project/Util/ExcelToJsonWizard.v1.0.6/excel_files/MonsterInfo.xlsx
+++ b/INFEST_Project/Util/ExcelToJsonWizard.v1.0.6/excel_files/MonsterInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\worni\Desktop\GitProject\INFEST\INFEST_Project\Util\ExcelToJsonWizard.v1.0.6\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62241C57-B174-4F76-B3F1-BF3549744E23}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08C5FFC-1C66-44EE-9122-F4A46CB0F230}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19245" windowHeight="8700" xr2:uid="{DE9B2C69-80EA-4400-AF84-1E72C6D3434C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="58">
   <si>
     <t>key</t>
   </si>
@@ -239,6 +239,10 @@
   </si>
   <si>
     <t>스폰수 제한</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SpeedMoveWave</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -651,10 +655,10 @@
   <sheetPr codeName="Sheet4">
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:T42"/>
+  <dimension ref="A1:U42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -672,16 +676,17 @@
     <col min="11" max="11" width="11.625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.75" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" customWidth="1"/>
-    <col min="14" max="14" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.25" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.25" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -722,28 +727,31 @@
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -792,20 +800,23 @@
       <c r="P2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="R2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="T2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="U2" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>21</v>
       </c>
@@ -846,28 +857,31 @@
         <v>33</v>
       </c>
       <c r="N3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="R3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S3" s="9" t="s">
+      <c r="T3" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="T3" s="9" t="s">
+      <c r="U3" s="9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1001</v>
       </c>
@@ -908,31 +922,34 @@
         <v>2</v>
       </c>
       <c r="M4">
-        <v>50</v>
+        <v>1.7</v>
       </c>
       <c r="N4">
+        <v>2.5</v>
+      </c>
+      <c r="O4">
         <v>0.7</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>5</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>100</v>
       </c>
-      <c r="Q4" s="5">
+      <c r="R4" s="5">
         <v>200</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>30</v>
       </c>
-      <c r="S4" t="b">
+      <c r="T4" t="b">
         <v>1</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>9999</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1002</v>
       </c>
@@ -973,31 +990,34 @@
         <v>2</v>
       </c>
       <c r="M5">
-        <v>60</v>
+        <v>1.9</v>
       </c>
       <c r="N5">
+        <v>2.8</v>
+      </c>
+      <c r="O5">
         <v>0.7</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>5</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>100</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="R5" s="5">
         <v>200</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>35</v>
       </c>
-      <c r="S5" t="b">
+      <c r="T5" t="b">
         <v>1</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>9999</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1003</v>
       </c>
@@ -1038,31 +1058,34 @@
         <v>2</v>
       </c>
       <c r="M6">
-        <v>70</v>
+        <v>2</v>
       </c>
       <c r="N6">
+        <v>3</v>
+      </c>
+      <c r="O6">
         <v>0.5</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>5</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>100</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="R6" s="5">
         <v>200</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>40</v>
       </c>
-      <c r="S6" t="b">
+      <c r="T6" t="b">
         <v>1</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>9999</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1004</v>
       </c>
@@ -1103,31 +1126,34 @@
         <v>2</v>
       </c>
       <c r="M7">
-        <v>65</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="N7">
+        <v>3.5</v>
+      </c>
+      <c r="O7">
         <v>0.65</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>5</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>100</v>
       </c>
-      <c r="Q7" s="5">
+      <c r="R7" s="5">
         <v>200</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>60</v>
       </c>
-      <c r="S7" t="b">
+      <c r="T7" t="b">
         <v>1</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>9999</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2001</v>
       </c>
@@ -1168,31 +1194,34 @@
         <v>4</v>
       </c>
       <c r="M8">
-        <v>65</v>
+        <v>1.8</v>
       </c>
       <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="O8">
         <v>0.7</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>4</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>13</v>
       </c>
-      <c r="Q8" s="5">
+      <c r="R8" s="5">
         <v>200</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>60</v>
       </c>
-      <c r="S8" t="b">
+      <c r="T8" t="b">
         <v>1</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>9999</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2002</v>
       </c>
@@ -1233,31 +1262,34 @@
         <v>4</v>
       </c>
       <c r="M9">
-        <v>80</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="N9">
+        <v>3.5</v>
+      </c>
+      <c r="O9">
         <v>0.85</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>7</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>100</v>
       </c>
-      <c r="Q9" s="5">
+      <c r="R9" s="5">
         <v>200</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>100</v>
       </c>
-      <c r="S9" t="b">
+      <c r="T9" t="b">
         <v>0</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>9999</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2003</v>
       </c>
@@ -1298,31 +1330,34 @@
         <v>4</v>
       </c>
       <c r="M10">
-        <v>75</v>
+        <v>2</v>
       </c>
       <c r="N10">
+        <v>3.2</v>
+      </c>
+      <c r="O10">
         <v>0.45</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>7</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>100</v>
       </c>
-      <c r="Q10" s="5">
+      <c r="R10" s="5">
         <v>200</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>100</v>
       </c>
-      <c r="S10" t="b">
+      <c r="T10" t="b">
         <v>0</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>9999</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3001</v>
       </c>
@@ -1362,31 +1397,34 @@
         <v>0</v>
       </c>
       <c r="M11">
-        <v>75</v>
+        <v>2.8</v>
       </c>
       <c r="N11">
+        <v>2.8</v>
+      </c>
+      <c r="O11">
         <v>0.8</v>
-      </c>
-      <c r="O11">
-        <v>15</v>
       </c>
       <c r="P11">
         <v>15</v>
       </c>
-      <c r="Q11" s="5">
+      <c r="Q11">
+        <v>15</v>
+      </c>
+      <c r="R11" s="5">
         <v>200</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>0</v>
       </c>
-      <c r="S11" t="b">
+      <c r="T11" t="b">
         <v>1</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3002</v>
       </c>
@@ -1426,31 +1464,34 @@
         <v>0</v>
       </c>
       <c r="M12">
-        <v>60</v>
+        <v>2.5</v>
       </c>
       <c r="N12">
+        <v>2.5</v>
+      </c>
+      <c r="O12">
         <v>0.6</v>
-      </c>
-      <c r="O12">
-        <v>15</v>
       </c>
       <c r="P12">
         <v>15</v>
       </c>
-      <c r="Q12" s="5">
+      <c r="Q12">
+        <v>15</v>
+      </c>
+      <c r="R12" s="5">
         <v>200</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>0</v>
       </c>
-      <c r="S12" t="b">
+      <c r="T12" t="b">
         <v>1</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -1466,8 +1507,9 @@
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="P14" s="6"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -1483,8 +1525,9 @@
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="P15" s="6"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1500,8 +1543,9 @@
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P16" s="6"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
@@ -1517,8 +1561,9 @@
       <c r="M17" s="6"/>
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P17" s="6"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -1534,8 +1579,9 @@
       <c r="M18" s="6"/>
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P18" s="6"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1551,8 +1597,9 @@
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P19" s="6"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -1568,8 +1615,9 @@
       <c r="M20" s="6"/>
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P20" s="6"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -1585,8 +1633,9 @@
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P21" s="6"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -1602,8 +1651,9 @@
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P22" s="6"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -1619,8 +1669,9 @@
       <c r="M23" s="6"/>
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P23" s="6"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -1636,8 +1687,9 @@
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P24" s="6"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -1653,8 +1705,9 @@
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P25" s="6"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -1670,8 +1723,9 @@
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P26" s="6"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -1687,8 +1741,9 @@
       <c r="M27" s="6"/>
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P27" s="6"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -1704,8 +1759,9 @@
       <c r="M28" s="6"/>
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P28" s="6"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -1721,8 +1777,9 @@
       <c r="M29" s="6"/>
       <c r="N29" s="6"/>
       <c r="O29" s="6"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P29" s="6"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -1738,8 +1795,9 @@
       <c r="M30" s="6"/>
       <c r="N30" s="6"/>
       <c r="O30" s="6"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P30" s="6"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -1755,8 +1813,9 @@
       <c r="M31" s="6"/>
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P31" s="6"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -1772,8 +1831,9 @@
       <c r="M32" s="6"/>
       <c r="N32" s="6"/>
       <c r="O32" s="6"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P32" s="6"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -1789,8 +1849,9 @@
       <c r="M33" s="6"/>
       <c r="N33" s="6"/>
       <c r="O33" s="6"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P33" s="6"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -1806,8 +1867,9 @@
       <c r="M34" s="6"/>
       <c r="N34" s="6"/>
       <c r="O34" s="6"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P34" s="6"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -1823,9 +1885,10 @@
       <c r="M35" s="6"/>
       <c r="N35" s="6"/>
       <c r="O35" s="6"/>
-    </row>
-    <row r="36" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P35" s="6"/>
+    </row>
+    <row r="36" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -1841,8 +1904,9 @@
       <c r="M37" s="6"/>
       <c r="N37" s="6"/>
       <c r="O37" s="6"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P37" s="6"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -1858,8 +1922,9 @@
       <c r="M38" s="6"/>
       <c r="N38" s="6"/>
       <c r="O38" s="6"/>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P38" s="6"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -1875,8 +1940,9 @@
       <c r="M39" s="6"/>
       <c r="N39" s="6"/>
       <c r="O39" s="6"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P39" s="6"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -1892,8 +1958,9 @@
       <c r="M40" s="6"/>
       <c r="N40" s="6"/>
       <c r="O40" s="6"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P40" s="6"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -1909,8 +1976,9 @@
       <c r="M41" s="6"/>
       <c r="N41" s="6"/>
       <c r="O41" s="6"/>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P41" s="6"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -1926,6 +1994,7 @@
       <c r="M42" s="6"/>
       <c r="N42" s="6"/>
       <c r="O42" s="6"/>
+      <c r="P42" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
feat: Add RageFang SkillData Table
</commit_message>
<xml_diff>
--- a/INFEST_Project/Util/ExcelToJsonWizard.v1.0.6/excel_files/MonsterInfo.xlsx
+++ b/INFEST_Project/Util/ExcelToJsonWizard.v1.0.6/excel_files/MonsterInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\worni\Desktop\GitProject\INFEST\INFEST_Project\Util\ExcelToJsonWizard.v1.0.6\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08C5FFC-1C66-44EE-9122-F4A46CB0F230}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A40609-E6D7-4155-BC89-1CC4BA6DE17D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19245" windowHeight="8700" xr2:uid="{DE9B2C69-80EA-4400-AF84-1E72C6D3434C}"/>
   </bookViews>
@@ -658,7 +658,7 @@
   <dimension ref="A1:U42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1409,7 +1409,7 @@
         <v>15</v>
       </c>
       <c r="Q11">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="R11" s="5">
         <v>200</v>
@@ -1476,7 +1476,7 @@
         <v>15</v>
       </c>
       <c r="Q12">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="R12" s="5">
         <v>200</v>

</xml_diff>

<commit_message>
fix: NavMesh 삭제(수정 예졍)
</commit_message>
<xml_diff>
--- a/INFEST_Project/Util/ExcelToJsonWizard.v1.0.6/excel_files/MonsterInfo.xlsx
+++ b/INFEST_Project/Util/ExcelToJsonWizard.v1.0.6/excel_files/MonsterInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\worni\Desktop\GitProject\INFEST\INFEST_Project\Util\ExcelToJsonWizard.v1.0.6\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0695FD-F19E-49ED-B367-B958B8E9EA02}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F1685B5-C0C8-40AE-9039-296E2D7205D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19245" windowHeight="8700" xr2:uid="{DE9B2C69-80EA-4400-AF84-1E72C6D3434C}"/>
   </bookViews>
@@ -689,7 +689,7 @@
   <dimension ref="A1:X42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:R12"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
fix: monster 이동속도 수정
</commit_message>
<xml_diff>
--- a/INFEST_Project/Util/ExcelToJsonWizard.v1.0.6/excel_files/MonsterInfo.xlsx
+++ b/INFEST_Project/Util/ExcelToJsonWizard.v1.0.6/excel_files/MonsterInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\worni\Desktop\GitProject\INFEST\INFEST_Project\Util\ExcelToJsonWizard.v1.0.6\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDD50D8-3D96-49FD-9484-7F434A2EE238}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD299D51-1BCD-4B9E-A11F-7E8711799184}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19245" windowHeight="8700" xr2:uid="{DE9B2C69-80EA-4400-AF84-1E72C6D3434C}"/>
   </bookViews>
@@ -690,8 +690,8 @@
   </sheetPr>
   <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -997,7 +997,7 @@
         <v>1.66</v>
       </c>
       <c r="Q4" s="10">
-        <v>2.48</v>
+        <v>4.5</v>
       </c>
       <c r="R4" s="10">
         <v>0.7</v>
@@ -1074,7 +1074,7 @@
         <v>1.66</v>
       </c>
       <c r="Q5" s="10">
-        <v>2.48</v>
+        <v>4.5</v>
       </c>
       <c r="R5" s="10">
         <v>0.7</v>
@@ -1151,7 +1151,7 @@
         <v>1.7</v>
       </c>
       <c r="Q6" s="10">
-        <v>2.4900000000000002</v>
+        <v>4.7</v>
       </c>
       <c r="R6" s="10">
         <v>0.5</v>
@@ -1228,7 +1228,7 @@
         <v>1.7</v>
       </c>
       <c r="Q7" s="10">
-        <v>2.5499999999999998</v>
+        <v>4.8</v>
       </c>
       <c r="R7" s="10">
         <v>0.65</v>
@@ -1305,7 +1305,7 @@
         <v>1.66</v>
       </c>
       <c r="Q8" s="10">
-        <v>2.4900000000000002</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="R8" s="10">
         <v>0.7</v>
@@ -1382,7 +1382,7 @@
         <v>2</v>
       </c>
       <c r="Q9" s="10">
-        <v>3</v>
+        <v>5.5</v>
       </c>
       <c r="R9" s="10">
         <v>0.85</v>
@@ -1459,7 +1459,7 @@
         <v>1.5</v>
       </c>
       <c r="Q10" s="10">
-        <v>2.25</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="R10" s="10">
         <v>0.45</v>

</xml_diff>

<commit_message>
fix: moster Move speed
</commit_message>
<xml_diff>
--- a/INFEST_Project/Util/ExcelToJsonWizard.v1.0.6/excel_files/MonsterInfo.xlsx
+++ b/INFEST_Project/Util/ExcelToJsonWizard.v1.0.6/excel_files/MonsterInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\worni\Desktop\GitProject\INFEST\INFEST_Project\Util\ExcelToJsonWizard.v1.0.6\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1D5B37-BB9B-4154-911D-57D6E5D97839}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3498BF6E-D182-452C-B37A-940DC230A8BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19245" windowHeight="8700" xr2:uid="{DE9B2C69-80EA-4400-AF84-1E72C6D3434C}"/>
   </bookViews>
@@ -693,8 +693,8 @@
   </sheetPr>
   <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4:P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -997,7 +997,7 @@
         <v>0.1</v>
       </c>
       <c r="P4" s="10">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="Q4" s="11">
         <v>11</v>
@@ -1074,7 +1074,7 @@
         <v>0.1</v>
       </c>
       <c r="P5" s="10">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="Q5" s="11">
         <v>12</v>
@@ -1151,7 +1151,7 @@
         <v>0.1</v>
       </c>
       <c r="P6" s="10">
-        <v>5.2</v>
+        <v>1.5</v>
       </c>
       <c r="Q6" s="11">
         <v>12</v>
@@ -1228,7 +1228,7 @@
         <v>0.1</v>
       </c>
       <c r="P7" s="10">
-        <v>5.3</v>
+        <v>1.5</v>
       </c>
       <c r="Q7" s="11">
         <v>13</v>
@@ -1305,7 +1305,7 @@
         <v>0.1</v>
       </c>
       <c r="P8" s="10">
-        <v>5.0999999999999996</v>
+        <v>1.5</v>
       </c>
       <c r="Q8" s="11">
         <v>12</v>
@@ -1382,7 +1382,7 @@
         <v>0.1</v>
       </c>
       <c r="P9" s="10">
-        <v>6</v>
+        <v>1.5</v>
       </c>
       <c r="Q9" s="11">
         <v>15</v>
@@ -1459,7 +1459,7 @@
         <v>0.1</v>
       </c>
       <c r="P10" s="10">
-        <v>4.9000000000000004</v>
+        <v>1.5</v>
       </c>
       <c r="Q10" s="11">
         <v>13</v>

</xml_diff>